<commit_message>
implements the feature of initialized display
</commit_message>
<xml_diff>
--- a/docs/dev_memo.xlsx
+++ b/docs/dev_memo.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="処理の構成" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="DAOの設計" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="例外処理" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="テキストの仕様と設計仕様の差分の対応" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t xml:space="preserve">項番</t>
   </si>
@@ -250,7 +251,10 @@
     <t xml:space="preserve">種別</t>
   </si>
   <si>
-    <t xml:space="preserve">DAOクラス</t>
+    <t xml:space="preserve">実装形式</t>
+  </si>
+  <si>
+    <t xml:space="preserve">実装するクラス</t>
   </si>
   <si>
     <t xml:space="preserve">スコープ</t>
@@ -268,7 +272,10 @@
     <t xml:space="preserve">共通</t>
   </si>
   <si>
-    <t xml:space="preserve">BaseDAO</t>
+    <t xml:space="preserve">継承</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daos</t>
   </si>
   <si>
     <t xml:space="preserve">protected</t>
@@ -280,6 +287,15 @@
     <t xml:space="preserve">void</t>
   </si>
   <si>
+    <t xml:space="preserve">servlets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gotoPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">リクエスト、レスポンス、遷移先URL</t>
+  </si>
+  <si>
     <t xml:space="preserve">非共通</t>
   </si>
   <si>
@@ -289,6 +305,12 @@
     <t xml:space="preserve">public</t>
   </si>
   <si>
+    <t xml:space="preserve">findAllCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">商品カテゴリーリスト</t>
+  </si>
+  <si>
     <t xml:space="preserve">findByCategory</t>
   </si>
   <si>
@@ -305,6 +327,9 @@
   </si>
   <si>
     <t xml:space="preserve">商品番号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　</t>
   </si>
   <si>
     <t xml:space="preserve">OrderDAO</t>
@@ -411,6 +436,136 @@
       </rPr>
       <t xml:space="preserve">において送出される例外を一括してエラー画面に遷移させる。</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">機能</t>
+  </si>
+  <si>
+    <t xml:space="preserve">サブ機能</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">機能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">サブ機能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">ID</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UC01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">初期画面表示</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">カート操作</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">商品追加</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内容表示</t>
+  </si>
+  <si>
+    <t xml:space="preserve">（カートから削除）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">商品削除</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">送付先入力</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">送付先確認</t>
+  </si>
+  <si>
+    <t xml:space="preserve">（顧客情報の登録）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">注文登録</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">送付先登録</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">注文伝票登録</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC0403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">注文明細登録</t>
   </si>
 </sst>
 </file>
@@ -512,7 +667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,12 +692,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -613,8 +788,7 @@
             <a:t>【脚註】</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -654,8 +828,7 @@
             <a:t>」になっている。</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -695,8 +868,7 @@
             <a:t>」になっている。</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -736,8 +908,7 @@
             <a:t>メソッド内で実行する。</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -798,8 +969,7 @@
             <a:t>【共通機能】</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -818,8 +988,7 @@
             <a:t>gotoPage(Request, Response, url)</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -894,8 +1063,7 @@
             <a:t>ショッピングサイトの改良</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -914,8 +1082,7 @@
             <a:t>：未入力の場合はエラー</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="メイリオ"/>
-            <a:ea typeface="メイリオ"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -932,7 +1099,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1250,21 +1417,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1286,103 +1454,153 @@
       <c r="F1" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:B8"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1416,63 +1634,63 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>79</v>
+      <c r="B1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>88</v>
+        <v>95</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1490,4 +1708,300 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.55078125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="8.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="8.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="13.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="9" width="16.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H12" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>